<commit_message>
Input file with degree and module final mark columns/rows
</commit_message>
<xml_diff>
--- a/Marks_template.xlsx
+++ b/Marks_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ginalamp/Workspace/ISM_SoftwareDev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EE79CB-897A-5E41-A575-47077F60D1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DCDA68-839F-884B-AA55-54191C9450CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="15720" xr2:uid="{DF5570C9-5617-A84F-92BB-2ECB05FFE319}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{DF5570C9-5617-A84F-92BB-2ECB05FFE319}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Advanced Information Systems Theory and Practice</t>
   </si>
@@ -66,7 +66,13 @@
     <t>Weight3 (%)</t>
   </si>
   <si>
-    <t>BComHons Information Systems Management</t>
+    <t>ModuleName</t>
+  </si>
+  <si>
+    <t>FinalModuleMark</t>
+  </si>
+  <si>
+    <t>Degree: BComHons Information Systems Management</t>
   </si>
 </sst>
 </file>
@@ -428,108 +434,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CDC4A8-45F7-CD43-A45C-A92B38F4D70F}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="49.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2">
+        <f>SUM(B3:B6)/COUNTA(B3:B6)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B3">
+        <f>C3*D3+E3*F3+G3*H3</f>
+        <v>75.5</v>
+      </c>
+      <c r="C3">
         <v>75</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D3" s="1">
         <v>0.5</v>
       </c>
-      <c r="D2">
+      <c r="E3">
         <v>75</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F3" s="1">
         <v>0.25</v>
       </c>
-      <c r="F2">
+      <c r="G3">
         <v>77</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H3" s="1">
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B4">
+        <f t="shared" ref="B4:B6" si="0">C4*D4+E4*F4+G4*H4</f>
+        <v>50</v>
+      </c>
+      <c r="C4">
         <v>100</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D4" s="1">
         <v>0.5</v>
       </c>
-      <c r="D3">
-        <v>70</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>86.5</v>
+      </c>
+      <c r="C5">
         <v>96</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D5" s="1">
         <v>0.5</v>
       </c>
-      <c r="D4">
+      <c r="E5">
         <v>77</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F5" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B6">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
csv may not have any spaces
</commit_message>
<xml_diff>
--- a/Marks_template.xlsx
+++ b/Marks_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ginalamp/Workspace/ISM_SoftwareDev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DCDA68-839F-884B-AA55-54191C9450CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E449E553-C281-D74F-819D-0472FC9F5736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{DF5570C9-5617-A84F-92BB-2ECB05FFE319}"/>
   </bookViews>
@@ -36,43 +36,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>Advanced Information Systems Theory and Practice</t>
-  </si>
-  <si>
-    <t>Computing in Information Systems</t>
-  </si>
-  <si>
-    <t>Information and Knowledge in Organisations</t>
-  </si>
-  <si>
-    <t>Research Assignment: Information Systems Management</t>
-  </si>
-  <si>
-    <t>Mark1 (%)</t>
-  </si>
-  <si>
-    <t>Mark2 (%)</t>
-  </si>
-  <si>
-    <t>Weight1 (%)</t>
-  </si>
-  <si>
-    <t>Weight2 (%)</t>
-  </si>
-  <si>
-    <t>Mark3 (%)</t>
-  </si>
-  <si>
-    <t>Weight3 (%)</t>
-  </si>
-  <si>
-    <t>ModuleName</t>
-  </si>
-  <si>
     <t>FinalModuleMark</t>
   </si>
   <si>
-    <t>Degree: BComHons Information Systems Management</t>
+    <t>Degree:BComHons_Information_Systems_Management</t>
+  </si>
+  <si>
+    <t>Module_Name</t>
+  </si>
+  <si>
+    <t>Mark1(%)</t>
+  </si>
+  <si>
+    <t>Weight1(%)</t>
+  </si>
+  <si>
+    <t>Mark2(%)</t>
+  </si>
+  <si>
+    <t>Weight2(%)</t>
+  </si>
+  <si>
+    <t>Mark3(%)</t>
+  </si>
+  <si>
+    <t>Weight3(%)</t>
+  </si>
+  <si>
+    <t>Advanced_Information_Systems_Theory_and_Practice</t>
+  </si>
+  <si>
+    <t>Computing_in_Information_Systems</t>
+  </si>
+  <si>
+    <t>Information_and_Knowledge_in_Organisations</t>
+  </si>
+  <si>
+    <t>Research_Assignment:_Information_Systems_Management</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,46 +451,47 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="2">
-        <f>SUM(B3:B6)/COUNTA(B3:B6)</f>
+        <v>1</v>
+      </c>
+      <c r="B1">
         <v>53</v>
       </c>
+      <c r="D1"/>
+      <c r="F1"/>
+      <c r="H1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <f>C3*D3+E3*F3+G3*H3</f>
-        <v>75.5</v>
+        <v>75</v>
       </c>
       <c r="C3">
         <v>75</v>
@@ -513,10 +514,9 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B6" si="0">C4*D4+E4*F4+G4*H4</f>
         <v>50</v>
       </c>
       <c r="C4">
@@ -531,14 +531,14 @@
       <c r="F4" s="1">
         <v>0.5</v>
       </c>
+      <c r="H4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>86.5</v>
+        <v>86</v>
       </c>
       <c r="C5">
         <v>96</v>
@@ -552,13 +552,13 @@
       <c r="F5" s="1">
         <v>0.5</v>
       </c>
+      <c r="H5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C6">
@@ -567,6 +567,8 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
+      <c r="F6"/>
+      <c r="H6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>